<commit_message>
nomina, subida tambien el de login
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alumno\Documents\NetBeansProjects\nomina\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alumno\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">actividades </t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Planificacion de proyecto nomina con BD</t>
+  </si>
+  <si>
+    <t>insertar login al programa</t>
   </si>
 </sst>
 </file>
@@ -72,7 +75,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +121,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -187,17 +196,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M22"/>
+  <dimension ref="A2:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,39 +501,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -559,10 +569,10 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -578,12 +588,12 @@
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -598,14 +608,14 @@
         <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -616,17 +626,17 @@
       <c r="A9" s="1">
         <v>4</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="11"/>
+      <c r="B9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="15"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -635,18 +645,18 @@
       <c r="A10" s="1">
         <v>5</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="11"/>
+      <c r="B10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="12"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
@@ -654,29 +664,29 @@
       <c r="A11" s="1">
         <v>6</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="11"/>
+      <c r="B11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="12"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="5"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="11"/>
+      <c r="B12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -685,15 +695,17 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="10"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -703,14 +715,14 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>9</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -726,8 +738,8 @@
       <c r="A15" s="1">
         <v>10</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -739,148 +751,22 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>11</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>12</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>13</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>14</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>15</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>16</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>17</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="D4:L4"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="F2:J2"/>
+  <mergeCells count="14">
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F2:J2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D4:L4"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>